<commit_message>
committing changed pom.xml, sirion admin.xml and deleted not required files and zip folder also removed and changed xls file to make a new working project
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Dashboard Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Dashboard Suite.xlsx
@@ -4,18 +4,21 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="Dashboard" sheetId="2" r:id="rId2"/>
+    <sheet name="Dashboard_Existing" sheetId="2" r:id="rId2"/>
+    <sheet name="Dashboard_new" sheetId="3" r:id="rId3"/>
+    <sheet name="Dashboard" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -57,15 +60,31 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>dashboardName</t>
+  </si>
+  <si>
+    <t>dashboardAnalyzeModeName</t>
+  </si>
+  <si>
+    <t>dashboardFilterModeName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,12 +144,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,16 +459,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="33.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,14 +512,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,7 +561,191 @@
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>4</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>

</xml_diff>

<commit_message>
commiting changes in Gaurav Branch for Dashboard Changes. change in following files changed: TestBase.java(wait time chnaged), config.properties(user id, url and browser type), Dashboard.java(all logic), TestSuiteBase.java(@after suite applied), Dashboard Suite.xlsx(new structure)
</commit_message>
<xml_diff>
--- a/src/test/resources/com/sirion/xls/Dashboard Suite.xlsx
+++ b/src/test/resources/com/sirion/xls/Dashboard Suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="5985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="5985" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,11 @@
     <sheet name="Dashboard" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G17"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="53">
   <si>
     <t>TCID</t>
   </si>
@@ -69,6 +68,114 @@
   </si>
   <si>
     <t>dashboardFilterModeName</t>
+  </si>
+  <si>
+    <t>Contract Status</t>
+  </si>
+  <si>
+    <t>Contract tcv</t>
+  </si>
+  <si>
+    <t>Actions - Overdue</t>
+  </si>
+  <si>
+    <t>Issues - Overdue</t>
+  </si>
+  <si>
+    <t>dashboardDownloadGraph</t>
+  </si>
+  <si>
+    <t>dashboardDownloadExcel</t>
+  </si>
+  <si>
+    <t>dashboardCategoryType</t>
+  </si>
+  <si>
+    <t>Invoice Volume</t>
+  </si>
+  <si>
+    <t>Contracts expiring in next 12 months (By Business Unit)</t>
+  </si>
+  <si>
+    <t>Perpetual Contracts</t>
+  </si>
+  <si>
+    <t>Contracts with Review Date in next 12 months (By Business Unit)</t>
+  </si>
+  <si>
+    <t>Contracts with Notice Date in next 12 months (By Business Unit)</t>
+  </si>
+  <si>
+    <t>Contracts expiring in next 12 months (By Supplier)</t>
+  </si>
+  <si>
+    <t>Contracts with Notice Date in next 12 months (By Supplier)</t>
+  </si>
+  <si>
+    <t>Contracts with Review Date in next 12 months (By Supplier)</t>
+  </si>
+  <si>
+    <t>SL Performance Trend</t>
+  </si>
+  <si>
+    <t>Function Services</t>
+  </si>
+  <si>
+    <t>TOP TEN SUPPLIERS- SL NOT MET (LAST 12 MONTHS)</t>
+  </si>
+  <si>
+    <t>Upcoming obligations</t>
+  </si>
+  <si>
+    <t>PO Burn by Spend Category</t>
+  </si>
+  <si>
+    <t>Spend Pool Analysis</t>
+  </si>
+  <si>
+    <t>SL Performance Tree</t>
+  </si>
+  <si>
+    <t>SL performance by geography</t>
+  </si>
+  <si>
+    <t>Open Actions Till Date</t>
+  </si>
+  <si>
+    <t>Open Issues Till Date</t>
+  </si>
+  <si>
+    <t>Open Obligations</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open Interpretation </t>
+  </si>
+  <si>
+    <t>Service Levels</t>
+  </si>
+  <si>
+    <t>Unpaid Invoices</t>
+  </si>
+  <si>
+    <t>Invoice Discrepancy</t>
+  </si>
+  <si>
+    <t>Credits &amp; Earnbacks</t>
+  </si>
+  <si>
+    <t>Open Policy Compliance</t>
+  </si>
+  <si>
+    <t>Service Levels Performance</t>
+  </si>
+  <si>
+    <t>Overdue Obligations</t>
+  </si>
+  <si>
+    <t>Change Request</t>
   </si>
 </sst>
 </file>
@@ -92,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +209,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -153,6 +266,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +580,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -581,10 +702,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -694,63 +815,657 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.140625" style="9" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="59.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="27.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12">
+        <v>2</v>
+      </c>
+      <c r="B2" s="14">
+        <v>17</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8">
+        <v>19</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8">
+        <v>20</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2</v>
+      </c>
+      <c r="B7" s="8">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>2</v>
+      </c>
+      <c r="B8" s="8">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2</v>
+      </c>
+      <c r="B9" s="8">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2</v>
+      </c>
+      <c r="B10" s="8">
+        <v>37</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2</v>
+      </c>
+      <c r="B11" s="8">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8">
+        <v>39</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2</v>
+      </c>
+      <c r="B13" s="8">
+        <v>47</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2</v>
+      </c>
+      <c r="B14" s="8">
+        <v>48</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2</v>
+      </c>
+      <c r="B15" s="8">
+        <v>49</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2</v>
+      </c>
+      <c r="B16" s="8">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>2</v>
+      </c>
+      <c r="B17" s="8">
+        <v>53</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>2</v>
+      </c>
+      <c r="B18" s="8">
+        <v>54</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>2</v>
+      </c>
+      <c r="B19" s="8">
+        <v>58</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>2</v>
+      </c>
+      <c r="B20" s="8">
+        <v>59</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1</v>
+      </c>
+      <c r="B21" s="11">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1</v>
+      </c>
+      <c r="B22" s="11">
+        <v>2</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1</v>
+      </c>
+      <c r="B23" s="11">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1</v>
+      </c>
+      <c r="B24" s="11">
+        <v>4</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="11">
+        <v>9</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1</v>
+      </c>
+      <c r="B26" s="11">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1</v>
+      </c>
+      <c r="B27" s="11">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1</v>
+      </c>
+      <c r="B28" s="11">
         <v>13</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
+      <c r="C28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1</v>
+      </c>
+      <c r="B29" s="11">
+        <v>14</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1</v>
+      </c>
+      <c r="B30" s="11">
+        <v>15</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1</v>
+      </c>
+      <c r="B31" s="11">
+        <v>16</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>1</v>
+      </c>
+      <c r="B32" s="11">
+        <v>21</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1</v>
+      </c>
+      <c r="B33" s="11">
+        <v>22</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1</v>
+      </c>
+      <c r="B34" s="11">
+        <v>36</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>